<commit_message>
Updated Habitat Quality pathway so attributes pull from LF pathway
</commit_message>
<xml_diff>
--- a/Output/Habitat_Quality_Scores.xlsx
+++ b/Output/Habitat_Quality_Scores.xlsx
@@ -23903,8 +23903,8 @@
       <c r="I299" t="e">
         <v>#N/A</v>
       </c>
-      <c r="J299" t="e">
-        <v>#N/A</v>
+      <c r="J299" t="n">
+        <v>3.0</v>
       </c>
       <c r="K299" t="e">
         <v>#N/A</v>
@@ -23918,8 +23918,8 @@
       <c r="N299" t="e">
         <v>#N/A</v>
       </c>
-      <c r="O299" t="e">
-        <v>#N/A</v>
+      <c r="O299" t="n">
+        <v>3.0</v>
       </c>
       <c r="P299" t="e">
         <v>#N/A</v>
@@ -23974,8 +23974,8 @@
       <c r="I300" t="e">
         <v>#N/A</v>
       </c>
-      <c r="J300" t="e">
-        <v>#N/A</v>
+      <c r="J300" t="n">
+        <v>3.0</v>
       </c>
       <c r="K300" t="e">
         <v>#N/A</v>
@@ -23989,8 +23989,8 @@
       <c r="N300" t="e">
         <v>#N/A</v>
       </c>
-      <c r="O300" t="e">
-        <v>#N/A</v>
+      <c r="O300" t="n">
+        <v>3.0</v>
       </c>
       <c r="P300" t="e">
         <v>#N/A</v>
@@ -50248,7 +50248,7 @@
         <v>5.0</v>
       </c>
       <c r="K670" t="n">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
       <c r="L670" t="n">
         <v>5.0</v>
@@ -50275,16 +50275,16 @@
         <v>2.0</v>
       </c>
       <c r="T670" t="n">
-        <v>41.0</v>
+        <v>37.0</v>
       </c>
       <c r="U670" t="n">
-        <v>0.9111111111111111</v>
+        <v>0.8222222222222222</v>
       </c>
       <c r="V670" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="W670" t="n">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="671">
@@ -54637,56 +54637,56 @@
       <c r="F732" t="s">
         <v>884</v>
       </c>
-      <c r="G732" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="H732" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="I732" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="J732" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="K732" t="e">
-        <v>#N/A</v>
+      <c r="G732" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H732" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="I732" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="J732" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="K732" t="n">
+        <v>1.0</v>
       </c>
       <c r="L732" t="n">
         <v>1.0</v>
       </c>
-      <c r="M732" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="N732" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="O732" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="P732" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="Q732" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="R732" t="e">
-        <v>#N/A</v>
+      <c r="M732" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="N732" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="O732" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="P732" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="Q732" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="R732" t="n">
+        <v>2.0</v>
       </c>
       <c r="S732" t="n">
         <v>3.0</v>
       </c>
-      <c r="T732" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="U732" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="V732" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="W732" t="e">
-        <v>#N/A</v>
+      <c r="T732" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="U732" t="n">
+        <v>0.35555555555555557</v>
+      </c>
+      <c r="V732" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="W732" t="n">
+        <v>1.0</v>
       </c>
     </row>
     <row r="733">
@@ -54708,56 +54708,56 @@
       <c r="F733" t="s">
         <v>884</v>
       </c>
-      <c r="G733" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="H733" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="I733" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="J733" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="K733" t="e">
-        <v>#N/A</v>
+      <c r="G733" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="H733" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="I733" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="J733" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="K733" t="n">
+        <v>3.0</v>
       </c>
       <c r="L733" t="n">
         <v>1.0</v>
       </c>
-      <c r="M733" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="N733" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="O733" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="P733" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="Q733" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="R733" t="e">
-        <v>#N/A</v>
+      <c r="M733" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="N733" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="O733" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="P733" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="Q733" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="R733" t="n">
+        <v>4.0</v>
       </c>
       <c r="S733" t="n">
         <v>3.0</v>
       </c>
-      <c r="T733" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="U733" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="V733" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="W733" t="e">
-        <v>#N/A</v>
+      <c r="T733" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="U733" t="n">
+        <v>0.6666666666666666</v>
+      </c>
+      <c r="V733" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="W733" t="n">
+        <v>1.0</v>
       </c>
     </row>
     <row r="734">
@@ -54779,56 +54779,56 @@
       <c r="F734" t="s">
         <v>884</v>
       </c>
-      <c r="G734" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="H734" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="I734" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="J734" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="K734" t="e">
-        <v>#N/A</v>
+      <c r="G734" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="H734" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="I734" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="J734" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="K734" t="n">
+        <v>5.0</v>
       </c>
       <c r="L734" t="n">
         <v>1.0</v>
       </c>
-      <c r="M734" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="N734" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="O734" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="P734" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="Q734" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="R734" t="e">
-        <v>#N/A</v>
+      <c r="M734" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="N734" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="O734" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="P734" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="Q734" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="R734" t="n">
+        <v>5.0</v>
       </c>
       <c r="S734" t="n">
         <v>3.0</v>
       </c>
-      <c r="T734" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="U734" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="V734" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="W734" t="e">
-        <v>#N/A</v>
+      <c r="T734" t="n">
+        <v>35.0</v>
+      </c>
+      <c r="U734" t="n">
+        <v>0.7777777777777778</v>
+      </c>
+      <c r="V734" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="W734" t="n">
+        <v>1.0</v>
       </c>
     </row>
     <row r="735">

</xml_diff>